<commit_message>
feat: Añadido codigo para el cargador de archivos
Codigo para que aparezca el cargador de archivos. Aun no funciona.
</commit_message>
<xml_diff>
--- a/programme-main-v9.xlsx
+++ b/programme-main-v9.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\program-manager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbc\Dropbox\investigacion\congresos\SPLC2017\Program\MAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11138" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Wednesday" sheetId="3" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="263">
   <si>
     <t>Wednesday, 27 Sep</t>
   </si>
@@ -880,9 +880,6 @@
   </si>
   <si>
     <t>TECHNICAL SESSIONS - parallel: Testing Product Lines (T3.2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Industry </t>
   </si>
 </sst>
 </file>
@@ -1329,16 +1326,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1378,92 +1365,102 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="86">
-    <cellStyle name="20% - Énfasis3" xfId="2" builtinId="38"/>
-    <cellStyle name="Énfasis5" xfId="1" builtinId="45"/>
-    <cellStyle name="Hipervínculo" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="16" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="18" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="20" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="22" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="24" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="26" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="28" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="30" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="32" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="34" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="36" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="38" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="40" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="42" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="56" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="58" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="60" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="62" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="64" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="66" builtinId="8"/>
-    <cellStyle name="Hipervínculo visitado" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
+    <cellStyle name="Accent5" xfId="1" builtinId="45"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
@@ -2129,56 +2126,56 @@
       <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="3" width="45.28515625" customWidth="1"/>
-    <col min="4" max="5" width="35.140625" customWidth="1"/>
+    <col min="2" max="3" width="45.33203125" customWidth="1"/>
+    <col min="4" max="5" width="35.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36"/>
-    </row>
-    <row r="2" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="33"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="41"/>
-    </row>
-    <row r="4" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="37"/>
+    </row>
+    <row r="4" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="C4" s="42"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="38"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="35"/>
-    </row>
-    <row r="6" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="31"/>
+    </row>
+    <row r="6" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>117</v>
       </c>
@@ -2189,16 +2186,16 @@
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="39"/>
-    </row>
-    <row r="8" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="35"/>
+    </row>
+    <row r="8" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>120</v>
       </c>
@@ -2209,52 +2206,52 @@
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="35"/>
-    </row>
-    <row r="10" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="31"/>
+    </row>
+    <row r="10" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="29" t="s">
         <v>240</v>
       </c>
-      <c r="C10" s="34"/>
-    </row>
-    <row r="11" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="30"/>
+    </row>
+    <row r="11" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="34"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="30"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="35"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="31"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="35"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="31"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="26"/>
     </row>
   </sheetData>
@@ -2292,47 +2289,47 @@
       <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="3" width="45.28515625" customWidth="1"/>
-    <col min="4" max="5" width="35.140625" customWidth="1"/>
+    <col min="2" max="3" width="45.33203125" customWidth="1"/>
+    <col min="4" max="5" width="35.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="B1" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="36"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="43"/>
-    </row>
-    <row r="3" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="39"/>
+    </row>
+    <row r="3" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="42"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="38"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="35"/>
-    </row>
-    <row r="5" spans="1:3" ht="64.349999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="31"/>
+    </row>
+    <row r="5" spans="1:3" ht="64.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>226</v>
       </c>
@@ -2343,34 +2340,34 @@
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="C6" s="35"/>
-    </row>
-    <row r="7" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="31"/>
+    </row>
+    <row r="7" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="C7" s="42"/>
-    </row>
-    <row r="8" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="38"/>
+    </row>
+    <row r="8" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="39"/>
-    </row>
-    <row r="9" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="35"/>
+    </row>
+    <row r="9" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -2381,23 +2378,23 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="C10" s="35"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="31"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="24" t="s">
         <v>245</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2432,29 +2429,29 @@
       <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="3" width="45.28515625" customWidth="1"/>
-    <col min="4" max="5" width="35.140625" customWidth="1"/>
+    <col min="2" max="3" width="45.33203125" customWidth="1"/>
+    <col min="4" max="5" width="35.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="43"/>
-    </row>
-    <row r="3" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="39"/>
+    </row>
+    <row r="3" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
@@ -2465,16 +2462,16 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="35"/>
-    </row>
-    <row r="5" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="31"/>
+    </row>
+    <row r="5" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -2485,33 +2482,33 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="45"/>
+      <c r="C6" s="41"/>
       <c r="D6" s="28"/>
     </row>
-    <row r="7" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="45"/>
-    </row>
-    <row r="8" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="41"/>
+    </row>
+    <row r="8" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="39"/>
+      <c r="C8" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2536,24 +2533,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="116.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="123.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="116.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="123.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -2591,7 +2588,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="7">
         <v>23</v>
       </c>
@@ -2629,7 +2626,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7">
         <v>35</v>
       </c>
@@ -2667,7 +2664,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7">
         <v>41</v>
       </c>
@@ -2705,7 +2702,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7">
         <v>84</v>
       </c>
@@ -2718,10 +2715,10 @@
       <c r="D5" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="45" t="s">
         <v>130</v>
       </c>
       <c r="G5" s="7" t="s">
@@ -2743,7 +2740,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7">
         <v>78</v>
       </c>
@@ -2756,10 +2753,10 @@
       <c r="D6" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="45" t="s">
         <v>227</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -2779,7 +2776,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7">
         <v>84</v>
       </c>
@@ -2815,7 +2812,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
         <v>90</v>
       </c>
@@ -2851,7 +2848,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="7">
         <v>91</v>
       </c>
@@ -2887,7 +2884,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
         <v>96</v>
       </c>
@@ -2923,7 +2920,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="7">
         <v>97</v>
       </c>
@@ -2959,7 +2956,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
         <v>98</v>
       </c>
@@ -2972,10 +2969,10 @@
       <c r="D12" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="44" t="s">
         <v>227</v>
       </c>
       <c r="G12" s="7" t="s">
@@ -2995,7 +2992,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7">
         <v>101</v>
       </c>
@@ -3011,7 +3008,7 @@
       <c r="E13" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="45" t="s">
         <v>227</v>
       </c>
       <c r="G13" s="7" t="s">
@@ -3031,7 +3028,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="7">
         <v>102</v>
       </c>
@@ -3067,7 +3064,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="7">
         <v>88</v>
       </c>
@@ -3103,7 +3100,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -3116,10 +3113,10 @@
       <c r="D16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="44" t="s">
         <v>224</v>
       </c>
       <c r="G16" s="7" t="s">
@@ -3141,7 +3138,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
         <v>21</v>
       </c>
@@ -3154,10 +3151,10 @@
       <c r="D17" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="44" t="s">
         <v>224</v>
       </c>
       <c r="G17" s="7" t="s">
@@ -3179,7 +3176,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="7">
         <v>98</v>
       </c>
@@ -3192,10 +3189,10 @@
       <c r="D18" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="44" t="s">
         <v>224</v>
       </c>
       <c r="G18" s="7" t="s">
@@ -3217,7 +3214,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="7">
         <v>42</v>
       </c>
@@ -3230,10 +3227,10 @@
       <c r="D19" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E19" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="44" t="s">
         <v>224</v>
       </c>
       <c r="G19" s="7" t="s">
@@ -3255,7 +3252,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="7">
         <v>22</v>
       </c>
@@ -3271,7 +3268,7 @@
       <c r="E20" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="44" t="s">
         <v>222</v>
       </c>
       <c r="G20" s="11" t="s">
@@ -3293,7 +3290,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="7">
         <v>54</v>
       </c>
@@ -3331,7 +3328,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="7">
         <v>5</v>
       </c>
@@ -3369,7 +3366,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="7">
         <v>50</v>
       </c>
@@ -3407,7 +3404,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
         <v>6</v>
       </c>
@@ -3445,7 +3442,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="7">
         <v>11</v>
       </c>
@@ -3483,7 +3480,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
         <v>91</v>
       </c>
@@ -3521,7 +3518,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="7">
         <v>97</v>
       </c>
@@ -3559,7 +3556,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="7">
         <v>8</v>
       </c>
@@ -3569,8 +3566,8 @@
       <c r="C28" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>263</v>
+      <c r="D28" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>133</v>
@@ -3597,7 +3594,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="7">
         <v>14</v>
       </c>
@@ -3635,7 +3632,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="7">
         <v>96</v>
       </c>
@@ -3673,7 +3670,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="7">
         <v>66</v>
       </c>
@@ -3689,7 +3686,7 @@
       <c r="E31" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="F31" s="29" t="s">
+      <c r="F31" s="42" t="s">
         <v>132</v>
       </c>
       <c r="G31" s="7" t="s">
@@ -3711,7 +3708,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="7">
         <v>9</v>
       </c>
@@ -3749,7 +3746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="7">
         <v>60</v>
       </c>
@@ -3787,7 +3784,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="7">
         <v>90</v>
       </c>
@@ -3825,7 +3822,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="15">
         <v>103</v>
       </c>
@@ -3863,7 +3860,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="7">
         <v>49</v>
       </c>
@@ -3901,7 +3898,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="7">
         <v>57</v>
       </c>
@@ -3939,7 +3936,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="7">
         <v>70</v>
       </c>
@@ -3952,10 +3949,10 @@
       <c r="D38" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="F38" s="32" t="s">
+      <c r="F38" s="45" t="s">
         <v>142</v>
       </c>
       <c r="G38" s="7" t="s">
@@ -3977,7 +3974,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="7">
         <v>102</v>
       </c>
@@ -3990,10 +3987,10 @@
       <c r="D39" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E39" s="30" t="s">
+      <c r="E39" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="F39" s="32" t="s">
+      <c r="F39" s="45" t="s">
         <v>142</v>
       </c>
       <c r="G39" s="7" t="s">
@@ -4015,7 +4012,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
         <v>25</v>
       </c>
@@ -4053,7 +4050,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="7">
         <v>30</v>
       </c>
@@ -4091,7 +4088,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
         <v>38</v>
       </c>
@@ -4129,7 +4126,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="7">
         <v>13</v>
       </c>
@@ -4167,7 +4164,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="7">
         <v>46</v>
       </c>
@@ -4205,7 +4202,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="7">
         <v>94</v>
       </c>
@@ -4218,10 +4215,10 @@
       <c r="D45" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E45" s="30" t="s">
+      <c r="E45" s="43" t="s">
         <v>219</v>
       </c>
-      <c r="F45" s="32" t="s">
+      <c r="F45" s="45" t="s">
         <v>140</v>
       </c>
       <c r="G45" s="7" t="s">
@@ -4243,7 +4240,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="7">
         <v>95</v>
       </c>
@@ -4259,7 +4256,7 @@
       <c r="E46" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="F46" s="30" t="s">
+      <c r="F46" s="43" t="s">
         <v>140</v>
       </c>
       <c r="G46" s="7" t="s">
@@ -4281,7 +4278,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="7">
         <v>108</v>
       </c>
@@ -4317,7 +4314,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="7">
         <v>109</v>
       </c>
@@ -4353,7 +4350,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="7">
         <v>110</v>
       </c>
@@ -4536,14 +4533,14 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="16" t="s">
         <v>215</v>
       </c>
@@ -4557,13 +4554,13 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>147</v>
       </c>
@@ -4575,7 +4572,7 @@
       </c>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>176</v>
       </c>
@@ -4587,7 +4584,7 @@
       </c>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>209</v>
       </c>
@@ -4599,7 +4596,7 @@
       </c>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="21" t="s">
         <v>203</v>
       </c>
@@ -4611,7 +4608,7 @@
       </c>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="19" t="s">
         <v>212</v>
       </c>
@@ -4623,7 +4620,7 @@
       </c>
       <c r="D7" s="22"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="19" t="s">
         <v>146</v>
       </c>
@@ -4635,7 +4632,7 @@
       </c>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="21" t="s">
         <v>206</v>
       </c>
@@ -4647,7 +4644,7 @@
       </c>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
         <v>179</v>
       </c>
@@ -4659,7 +4656,7 @@
       </c>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="21" t="s">
         <v>185</v>
       </c>
@@ -4671,7 +4668,7 @@
       </c>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
         <v>156</v>
       </c>
@@ -4683,7 +4680,7 @@
       </c>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="21" t="s">
         <v>173</v>
       </c>
@@ -4695,7 +4692,7 @@
       </c>
       <c r="D13" s="18"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="19" t="s">
         <v>200</v>
       </c>
@@ -4707,7 +4704,7 @@
       </c>
       <c r="D14" s="18"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="21" t="s">
         <v>197</v>
       </c>
@@ -4719,7 +4716,7 @@
       </c>
       <c r="D15" s="18"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="19" t="s">
         <v>194</v>
       </c>
@@ -4731,7 +4728,7 @@
       </c>
       <c r="D16" s="18"/>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="21" t="s">
         <v>170</v>
       </c>
@@ -4743,7 +4740,7 @@
       </c>
       <c r="D17" s="18"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="21" t="s">
         <v>150</v>
       </c>
@@ -4755,7 +4752,7 @@
       </c>
       <c r="D18" s="18"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="21" t="s">
         <v>167</v>
       </c>
@@ -4767,7 +4764,7 @@
       </c>
       <c r="D19" s="23"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="21" t="s">
         <v>164</v>
       </c>
@@ -4779,7 +4776,7 @@
       </c>
       <c r="D20" s="18"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="21" t="s">
         <v>159</v>
       </c>
@@ -4791,7 +4788,7 @@
       </c>
       <c r="D21" s="18"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="21" t="s">
         <v>153</v>
       </c>
@@ -4803,7 +4800,7 @@
       </c>
       <c r="D22" s="18"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="21" t="s">
         <v>188</v>
       </c>
@@ -4815,7 +4812,7 @@
       </c>
       <c r="D23" s="18"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="19" t="s">
         <v>182</v>
       </c>
@@ -4827,7 +4824,7 @@
       </c>
       <c r="D24" s="18"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="19" t="s">
         <v>191</v>
       </c>

</xml_diff>

<commit_message>
doc: Actualización de archivos
Se procede a actualizar todos los archivos de la rama master.
</commit_message>
<xml_diff>
--- a/programme-main-v9.xlsx
+++ b/programme-main-v9.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbc\Dropbox\investigacion\congresos\SPLC2017\Program\MAIN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\program-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11138" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Wednesday" sheetId="3" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="264">
   <si>
     <t>Wednesday, 27 Sep</t>
   </si>
@@ -880,6 +880,9 @@
   </si>
   <si>
     <t>TECHNICAL SESSIONS - parallel: Testing Product Lines (T3.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industry </t>
   </si>
 </sst>
 </file>
@@ -1326,6 +1329,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1365,102 +1378,92 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="86">
-    <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
-    <cellStyle name="Accent5" xfId="1" builtinId="45"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="66" builtinId="8"/>
+    <cellStyle name="20% - Énfasis3" xfId="2" builtinId="38"/>
+    <cellStyle name="Énfasis5" xfId="1" builtinId="45"/>
+    <cellStyle name="Hipervínculo" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="66" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
@@ -2126,56 +2129,56 @@
       <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="3" width="45.33203125" customWidth="1"/>
-    <col min="4" max="5" width="35.1328125" customWidth="1"/>
+    <col min="2" max="3" width="45.28515625" customWidth="1"/>
+    <col min="4" max="5" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="B1" s="32" t="s">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
-    </row>
-    <row r="2" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="33"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C2" s="37"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="40" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="37"/>
-    </row>
-    <row r="4" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C3" s="41"/>
+    </row>
+    <row r="4" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="33" t="s">
         <v>231</v>
       </c>
-      <c r="C4" s="38"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C4" s="42"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="31"/>
-    </row>
-    <row r="6" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C5" s="35"/>
+    </row>
+    <row r="6" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>117</v>
       </c>
@@ -2186,16 +2189,16 @@
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="35"/>
-    </row>
-    <row r="8" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C7" s="39"/>
+    </row>
+    <row r="8" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>120</v>
       </c>
@@ -2206,52 +2209,52 @@
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="31"/>
-    </row>
-    <row r="10" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="35"/>
+    </row>
+    <row r="10" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="33" t="s">
         <v>240</v>
       </c>
-      <c r="C10" s="30"/>
-    </row>
-    <row r="11" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C10" s="34"/>
+    </row>
+    <row r="11" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="30"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C11" s="34"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="31"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C12" s="35"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="31"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C13" s="35"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
     </row>
   </sheetData>
@@ -2289,47 +2292,47 @@
       <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="3" width="45.33203125" customWidth="1"/>
-    <col min="4" max="5" width="35.1328125" customWidth="1"/>
+    <col min="2" max="3" width="45.28515625" customWidth="1"/>
+    <col min="4" max="5" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="B1" s="32" t="s">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="32"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="39"/>
-    </row>
-    <row r="3" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="43"/>
+    </row>
+    <row r="3" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="38"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C3" s="42"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="31"/>
-    </row>
-    <row r="5" spans="1:3" ht="64.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C4" s="35"/>
+    </row>
+    <row r="5" spans="1:3" ht="64.349999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>226</v>
       </c>
@@ -2340,34 +2343,34 @@
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="35" t="s">
         <v>251</v>
       </c>
-      <c r="C6" s="31"/>
-    </row>
-    <row r="7" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C6" s="35"/>
+    </row>
+    <row r="7" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="33" t="s">
         <v>221</v>
       </c>
-      <c r="C7" s="38"/>
-    </row>
-    <row r="8" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C7" s="42"/>
+    </row>
+    <row r="8" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="35"/>
-    </row>
-    <row r="9" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="39"/>
+    </row>
+    <row r="9" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -2378,23 +2381,23 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="C10" s="31"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C10" s="35"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>245</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="C11" s="31"/>
+      <c r="C11" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2429,29 +2432,29 @@
       <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="3" width="45.33203125" customWidth="1"/>
-    <col min="4" max="5" width="35.1328125" customWidth="1"/>
+    <col min="2" max="3" width="45.28515625" customWidth="1"/>
+    <col min="4" max="5" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="B1" s="32" t="s">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="39"/>
-    </row>
-    <row r="3" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="43"/>
+    </row>
+    <row r="3" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
@@ -2462,16 +2465,16 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="31"/>
-    </row>
-    <row r="5" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C4" s="35"/>
+    </row>
+    <row r="5" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -2482,33 +2485,33 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="28"/>
     </row>
-    <row r="7" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="41"/>
-    </row>
-    <row r="8" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C7" s="45"/>
+    </row>
+    <row r="8" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="35"/>
+      <c r="C8" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2533,24 +2536,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="116.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="123.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="116.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="123.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -2588,7 +2591,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>23</v>
       </c>
@@ -2626,7 +2629,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>35</v>
       </c>
@@ -2664,7 +2667,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>41</v>
       </c>
@@ -2702,7 +2705,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>84</v>
       </c>
@@ -2715,10 +2718,10 @@
       <c r="D5" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="F5" s="45" t="s">
+      <c r="F5" s="32" t="s">
         <v>130</v>
       </c>
       <c r="G5" s="7" t="s">
@@ -2740,7 +2743,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>78</v>
       </c>
@@ -2753,10 +2756,10 @@
       <c r="D6" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="F6" s="45" t="s">
+      <c r="F6" s="32" t="s">
         <v>227</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -2776,7 +2779,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>84</v>
       </c>
@@ -2812,7 +2815,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>90</v>
       </c>
@@ -2848,7 +2851,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>91</v>
       </c>
@@ -2884,7 +2887,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>96</v>
       </c>
@@ -2920,7 +2923,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>97</v>
       </c>
@@ -2956,7 +2959,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>98</v>
       </c>
@@ -2969,10 +2972,10 @@
       <c r="D12" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="31" t="s">
         <v>227</v>
       </c>
       <c r="G12" s="7" t="s">
@@ -2992,7 +2995,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>101</v>
       </c>
@@ -3008,7 +3011,7 @@
       <c r="E13" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="F13" s="45" t="s">
+      <c r="F13" s="32" t="s">
         <v>227</v>
       </c>
       <c r="G13" s="7" t="s">
@@ -3028,7 +3031,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>102</v>
       </c>
@@ -3064,7 +3067,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>88</v>
       </c>
@@ -3100,7 +3103,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -3113,10 +3116,10 @@
       <c r="D16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="F16" s="44" t="s">
+      <c r="F16" s="31" t="s">
         <v>224</v>
       </c>
       <c r="G16" s="7" t="s">
@@ -3138,7 +3141,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>21</v>
       </c>
@@ -3151,10 +3154,10 @@
       <c r="D17" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="F17" s="44" t="s">
+      <c r="F17" s="31" t="s">
         <v>224</v>
       </c>
       <c r="G17" s="7" t="s">
@@ -3176,7 +3179,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>98</v>
       </c>
@@ -3189,10 +3192,10 @@
       <c r="D18" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="F18" s="31" t="s">
         <v>224</v>
       </c>
       <c r="G18" s="7" t="s">
@@ -3214,7 +3217,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>42</v>
       </c>
@@ -3227,10 +3230,10 @@
       <c r="D19" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="F19" s="44" t="s">
+      <c r="F19" s="31" t="s">
         <v>224</v>
       </c>
       <c r="G19" s="7" t="s">
@@ -3252,7 +3255,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>22</v>
       </c>
@@ -3268,7 +3271,7 @@
       <c r="E20" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="F20" s="44" t="s">
+      <c r="F20" s="31" t="s">
         <v>222</v>
       </c>
       <c r="G20" s="11" t="s">
@@ -3290,7 +3293,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>54</v>
       </c>
@@ -3328,7 +3331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>5</v>
       </c>
@@ -3366,7 +3369,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>50</v>
       </c>
@@ -3404,7 +3407,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>6</v>
       </c>
@@ -3442,7 +3445,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>11</v>
       </c>
@@ -3480,7 +3483,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>91</v>
       </c>
@@ -3518,7 +3521,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>97</v>
       </c>
@@ -3556,7 +3559,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>8</v>
       </c>
@@ -3566,8 +3569,8 @@
       <c r="C28" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>37</v>
+      <c r="D28" s="11" t="s">
+        <v>263</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>133</v>
@@ -3594,7 +3597,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>14</v>
       </c>
@@ -3632,7 +3635,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>96</v>
       </c>
@@ -3670,7 +3673,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>66</v>
       </c>
@@ -3686,7 +3689,7 @@
       <c r="E31" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="F31" s="42" t="s">
+      <c r="F31" s="29" t="s">
         <v>132</v>
       </c>
       <c r="G31" s="7" t="s">
@@ -3708,7 +3711,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>9</v>
       </c>
@@ -3746,7 +3749,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>60</v>
       </c>
@@ -3784,7 +3787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>90</v>
       </c>
@@ -3822,7 +3825,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>103</v>
       </c>
@@ -3860,7 +3863,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>49</v>
       </c>
@@ -3898,7 +3901,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>57</v>
       </c>
@@ -3936,7 +3939,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>70</v>
       </c>
@@ -3949,10 +3952,10 @@
       <c r="D38" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="43" t="s">
+      <c r="E38" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="F38" s="45" t="s">
+      <c r="F38" s="32" t="s">
         <v>142</v>
       </c>
       <c r="G38" s="7" t="s">
@@ -3974,7 +3977,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>102</v>
       </c>
@@ -3987,10 +3990,10 @@
       <c r="D39" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E39" s="43" t="s">
+      <c r="E39" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="F39" s="45" t="s">
+      <c r="F39" s="32" t="s">
         <v>142</v>
       </c>
       <c r="G39" s="7" t="s">
@@ -4012,7 +4015,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>25</v>
       </c>
@@ -4050,7 +4053,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>30</v>
       </c>
@@ -4088,7 +4091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>38</v>
       </c>
@@ -4126,7 +4129,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>13</v>
       </c>
@@ -4164,7 +4167,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>46</v>
       </c>
@@ -4202,7 +4205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>94</v>
       </c>
@@ -4215,10 +4218,10 @@
       <c r="D45" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E45" s="43" t="s">
+      <c r="E45" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="F45" s="45" t="s">
+      <c r="F45" s="32" t="s">
         <v>140</v>
       </c>
       <c r="G45" s="7" t="s">
@@ -4240,7 +4243,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>95</v>
       </c>
@@ -4256,7 +4259,7 @@
       <c r="E46" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="F46" s="43" t="s">
+      <c r="F46" s="30" t="s">
         <v>140</v>
       </c>
       <c r="G46" s="7" t="s">
@@ -4278,7 +4281,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>108</v>
       </c>
@@ -4314,7 +4317,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>109</v>
       </c>
@@ -4350,7 +4353,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>110</v>
       </c>
@@ -4533,14 +4536,14 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>215</v>
       </c>
@@ -4554,13 +4557,13 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>147</v>
       </c>
@@ -4572,7 +4575,7 @@
       </c>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>176</v>
       </c>
@@ -4584,7 +4587,7 @@
       </c>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>209</v>
       </c>
@@ -4596,7 +4599,7 @@
       </c>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>203</v>
       </c>
@@ -4608,7 +4611,7 @@
       </c>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>212</v>
       </c>
@@ -4620,7 +4623,7 @@
       </c>
       <c r="D7" s="22"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>146</v>
       </c>
@@ -4632,7 +4635,7 @@
       </c>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>206</v>
       </c>
@@ -4644,7 +4647,7 @@
       </c>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>179</v>
       </c>
@@ -4656,7 +4659,7 @@
       </c>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>185</v>
       </c>
@@ -4668,7 +4671,7 @@
       </c>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>156</v>
       </c>
@@ -4680,7 +4683,7 @@
       </c>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>173</v>
       </c>
@@ -4692,7 +4695,7 @@
       </c>
       <c r="D13" s="18"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>200</v>
       </c>
@@ -4704,7 +4707,7 @@
       </c>
       <c r="D14" s="18"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>197</v>
       </c>
@@ -4716,7 +4719,7 @@
       </c>
       <c r="D15" s="18"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>194</v>
       </c>
@@ -4728,7 +4731,7 @@
       </c>
       <c r="D16" s="18"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>170</v>
       </c>
@@ -4740,7 +4743,7 @@
       </c>
       <c r="D17" s="18"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>150</v>
       </c>
@@ -4752,7 +4755,7 @@
       </c>
       <c r="D18" s="18"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>167</v>
       </c>
@@ -4764,7 +4767,7 @@
       </c>
       <c r="D19" s="23"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>164</v>
       </c>
@@ -4776,7 +4779,7 @@
       </c>
       <c r="D20" s="18"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>159</v>
       </c>
@@ -4788,7 +4791,7 @@
       </c>
       <c r="D21" s="18"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>153</v>
       </c>
@@ -4800,7 +4803,7 @@
       </c>
       <c r="D22" s="18"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>188</v>
       </c>
@@ -4812,7 +4815,7 @@
       </c>
       <c r="D23" s="18"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>182</v>
       </c>
@@ -4824,7 +4827,7 @@
       </c>
       <c r="D24" s="18"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>191</v>
       </c>

</xml_diff>